<commit_message>
Made a mistake in the call to the lac2pks function and fixed it
</commit_message>
<xml_diff>
--- a/AIC9parameters_bound4.xlsx
+++ b/AIC9parameters_bound4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FC775B-AB74-4D14-AD9F-8BF108A3B08A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF5993C-BAE4-4BAC-86ED-0CF3009F8353}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{366C0DC8-E829-4FAD-9D11-4CD559E70211}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{366C0DC8-E829-4FAD-9D11-4CD559E70211}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,182 +383,182 @@
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2204.2292171864119</v>
+        <v>2204.2292172112393</v>
       </c>
       <c r="B1">
-        <v>1385.8249072685196</v>
+        <v>1386.0864356158613</v>
       </c>
       <c r="C1">
-        <v>1434.5268945738233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1434.8848532135837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2227.119236892242</v>
+        <v>2227.1192368922416</v>
       </c>
       <c r="B2">
-        <v>1482.0443111325599</v>
+        <v>1482.0442356022584</v>
       </c>
       <c r="C2">
-        <v>1329.6420308346146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1329.6420231576942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.9137069401986</v>
+        <v>2343.9137069401977</v>
       </c>
       <c r="B3">
-        <v>1532.1749237175711</v>
+        <v>1532.1749178163932</v>
       </c>
       <c r="C3">
-        <v>1629.9765789738558</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1629.9765938678086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625294467764</v>
+        <v>2320.9625339441868</v>
       </c>
       <c r="B4">
-        <v>1791.2931533693336</v>
+        <v>1791.2092367794739</v>
       </c>
       <c r="C4">
-        <v>1735.3767825141572</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1735.3768306211518</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6539933912654</v>
+        <v>2422.6539933918984</v>
       </c>
       <c r="B5">
-        <v>1663.7700884670039</v>
+        <v>1663.7700490803886</v>
       </c>
       <c r="C5">
-        <v>1643.2197904604604</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1643.2199901288009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.708546824399</v>
+        <v>2360.7085097391273</v>
       </c>
       <c r="B6">
-        <v>1776.1845810515506</v>
+        <v>1775.9546966267449</v>
       </c>
       <c r="C6">
-        <v>1784.672455274761</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1784.4483163994612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9864161741264</v>
+        <v>1992.9864161485818</v>
       </c>
       <c r="B7">
-        <v>1556.0413514396798</v>
+        <v>1556.0441516909277</v>
       </c>
       <c r="C7">
-        <v>1533.383976106607</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1533.3702716577748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.7478413983877</v>
+        <v>2135.7478628495105</v>
       </c>
       <c r="B8">
-        <v>1655.7249330385901</v>
+        <v>1655.7390017928153</v>
       </c>
       <c r="C8">
-        <v>1507.3221427558281</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1507.358482697219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2471.0153725375085</v>
       </c>
       <c r="B9">
-        <v>1788.9602503559245</v>
+        <v>1788.9612874546681</v>
       </c>
       <c r="C9">
-        <v>1515.4110391951399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1515.4135845837143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.5944046572426</v>
+        <v>2111.59440425195</v>
       </c>
       <c r="B10">
-        <v>1364.6411889079691</v>
+        <v>1363.7332583996726</v>
       </c>
       <c r="C10">
-        <v>1302.0903149616599</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1304.7589921853487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1970.0041216261243</v>
+        <v>1970.0041216250017</v>
       </c>
       <c r="B11">
-        <v>1414.799188154708</v>
+        <v>1414.7991874097338</v>
       </c>
       <c r="C11">
-        <v>1308.3661889304565</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1308.366163587184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.9537212072742</v>
+        <v>2787.9537212083187</v>
       </c>
       <c r="B12">
-        <v>2270.4390872549134</v>
+        <v>2270.4390871133605</v>
       </c>
       <c r="C12">
-        <v>2036.7338403258118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2036.7338423286046</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2315.1853410978001</v>
       </c>
       <c r="B13">
-        <v>1763.9087267545681</v>
+        <v>1763.9087267538075</v>
       </c>
       <c r="C13">
-        <v>1803.6382322342629</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1803.6382322348347</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0481329755003</v>
+        <v>2593.0481324833731</v>
       </c>
       <c r="B14">
-        <v>1922.4486894831293</v>
+        <v>1922.4492006468518</v>
       </c>
       <c r="C14">
-        <v>1703.8062897316559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1703.8047046772597</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.4810607047993</v>
+        <v>2508.5108802462019</v>
       </c>
       <c r="B15">
-        <v>2024.669190140949</v>
+        <v>2026.7229049020305</v>
       </c>
       <c r="C15">
-        <v>1824.8884967725385</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1827.5083485611945</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.5222329985186</v>
+        <v>2205.5222145157363</v>
       </c>
       <c r="B16">
-        <v>1512.7080755521226</v>
+        <v>1512.621046798469</v>
       </c>
       <c r="C16">
-        <v>1379.4588586115867</v>
+        <v>1374.8836059549424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>